<commit_message>
added spaces in author name etc
</commit_message>
<xml_diff>
--- a/selfPublishing data.xlsx
+++ b/selfPublishing data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="19155" windowHeight="10050" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="19155" windowHeight="10050" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -459,43 +459,43 @@
     <t>Cover and Production</t>
   </si>
   <si>
-    <t>http://10.1.6.32/selfpublishing/get_method.php?companyId=11829044757&amp;groupId=11829076861&amp;bookInfo=%7B%22AuthorName%22%3A%20%22John%20Doe%22%2C%22Email%22%3A%20%22JD%40gmail.com%22%2C%22ISBN%22%3A%20%22%22%2C%22Cover%22%3A%20%22Color%22%2C%22Editorial%20Complexity%22%3A%20%22Low%22%2C%22NumberofManuscriptPages%22%3A%20%22251%22%7D&amp;redirectURL=https://www.pagemajik.com/&amp;bookDetails=%7B%22categoryName%22%3A%22Cover%20Design%22%2C%22bookName%22%3A%22%20Arbitration%20%26%20Conciliation%20%22%2C%22chapterCount%22%3A%222%22%2C%20%22isCoverDesignOnly%22%3A%22true%22%7D&amp;userDetails=%7B%22firstName%22%3A%20%22Sulthana%22%2C%22surName%22%3A%20%22S%22%2C%22mailId%22%3A%20%22sulthanas%40s4carlisle.com%22%20%7D</t>
-  </si>
-  <si>
-    <t>http://10.1.6.32/selfpublishing/get_method.php?companyId=11829044757&amp;groupId=11829076861&amp;bookInfo=%7B%22AuthorName%22%3A%20%22John%20Doe%22%2C%22Email%22%3A%20%22JD%40gmail.com%22%2C%22ISBN%22%3A%20%22%22%2C%22Cover%22%3A%20%22Color%22%2C%22Editorial%20Complexity%22%3A%20%22Low%22%2C%22NumberofManuscriptPages%22%3A%20%22251%22%7D&amp;redirectURL=https://www.pagemajik.com/&amp;bookDetails=%7B%22categoryName%22%3A%22Production%20Services%22%2C%22bookName%22%3A%22%20Arbitration%20%26%20Conciliation%20%22%2C%22chapterCount%22%3A%222%22%2C%20%22isCoverDesignOnly%22%3A%22true%22%7D&amp;userDetails=%7B%22firstName%22%3A%20%22Sulthana%22%2C%22surName%22%3A%20%22S%22%2C%22mailId%22%3A%20%22sulthanas%40s4carlisle.com%22%20%7D</t>
-  </si>
-  <si>
-    <t>http://10.1.6.32/selfpublishing/get_method.php?companyId=11829044757&amp;groupId=11829076861&amp;bookInfo=%7B%22AuthorName%22%3A%20%22John%20Doe%22%2C%22Email%22%3A%20%22JD%40gmail.com%22%2C%22ISBN%22%3A%20%22%22%2C%22Cover%22%3A%20%22Color%22%2C%22Editorial%20Complexity%22%3A%20%22Low%22%2C%22NumberofManuscriptPages%22%3A%20%22251%22%7D&amp;redirectURL=https://www.pagemajik.com/&amp;bookDetails=%7B%22categoryName%22%3A%22Editorial%20Services%22%2C%22bookName%22%3A%22%20Arbitration%20%26%20Conciliation%20%22%2C%22chapterCount%22%3A%222%22%2C%20%22isCoverDesignOnly%22%3A%22true%22%7D&amp;userDetails=%7B%22firstName%22%3A%20%22Sulthana%22%2C%22surName%22%3A%20%22S%22%2C%22mailId%22%3A%20%22sulthanas%40s4carlisle.com%22%20%7D</t>
-  </si>
-  <si>
-    <t>http://10.1.6.32/selfpublishing/get_method.php?companyId=11829044757&amp;groupId=11829076861&amp;bookInfo=%7B%22AuthorName%22%3A%20%22John%20Doe%22%2C%22Email%22%3A%20%22JD%40gmail.com%22%2C%22ISBN%22%3A%20%22%22%2C%22Cover%22%3A%20%22Color%22%2C%22Editorial%20Complexity%22%3A%20%22Low%22%2C%22NumberofManuscriptPages%22%3A%20%22251%22%7D&amp;redirectURL=https://www.pagemajik.com/&amp;bookDetails=%7B%22categoryName%22%3A%22Full%20Services%22%2C%22bookName%22%3A%22%20Arbitration%20%26%20Conciliation%20%22%2C%22chapterCount%22%3A%222%22%2C%20%22isCoverDesignOnly%22%3A%22true%22%7D&amp;userDetails=%7B%22firstName%22%3A%20%22Sulthana%22%2C%22surName%22%3A%20%22S%22%2C%22mailId%22%3A%20%22sulthanas%40s4carlisle.com%22%20%7D</t>
-  </si>
-  <si>
-    <t>http://10.1.6.32/selfpublishing/get_method.php?companyId=11829044757&amp;groupId=11829076861&amp;bookInfo=%7B%22AuthorName%22%3A%20%22John%20Doe%22%2C%22Email%22%3A%20%22JD%40gmail.com%22%2C%22ISBN%22%3A%20%22%22%2C%22Cover%22%3A%20%22Color%22%2C%22Editorial%20Complexity%22%3A%20%22Low%22%2C%22NumberofManuscriptPages%22%3A%20%22251%22%7D&amp;redirectURL=https://www.pagemajik.com/&amp;bookDetails=%7B%22categoryName%22%3A%22Index%22%2C%22bookName%22%3A%22%20Arbitration%20%26%20Conciliation%20%22%2C%22chapterCount%22%3A%222%22%2C%20%22isCoverDesignOnly%22%3A%22true%22%7D&amp;userDetails=%7B%22firstName%22%3A%20%22Sulthana%22%2C%22surName%22%3A%20%22S%22%2C%22mailId%22%3A%20%22sulthanas%40s4carlisle.com%22%20%7D</t>
-  </si>
-  <si>
-    <t>http://10.1.6.32/selfpublishing/get_method.php?companyId=11829044757&amp;groupId=11829076861&amp;bookInfo=%7B%22AuthorName%22%3A%20%22John%20Doe%22%2C%22Email%22%3A%20%22JD%40gmail.com%22%2C%22ISBN%22%3A%20%22%22%2C%22Cover%22%3A%20%22Color%22%2C%22Editorial%20Complexity%22%3A%20%22Low%22%2C%22NumberofManuscriptPages%22%3A%20%22251%22%7D&amp;redirectURL=https://www.pagemajik.com/&amp;bookDetails=%7B%22categoryName%22%3A%22Production%20and%20Index%22%2C%22bookName%22%3A%22%20Arbitration%20%26%20Conciliation%20%22%2C%22chapterCount%22%3A%222%22%2C%20%22isCoverDesignOnly%22%3A%22true%22%7D&amp;userDetails=%7B%22firstName%22%3A%20%22Sulthana%22%2C%22surName%22%3A%20%22S%22%2C%22mailId%22%3A%20%22sulthanas%40s4carlisle.com%22%20%7D</t>
-  </si>
-  <si>
-    <t>http://10.1.6.32/selfpublishing/get_method.php?companyId=11829044757&amp;groupId=11829076861&amp;bookInfo=%7B%22AuthorName%22%3A%20%22John%20Doe%22%2C%22Email%22%3A%20%22JD%40gmail.com%22%2C%22ISBN%22%3A%20%22%22%2C%22Cover%22%3A%20%22Color%22%2C%22Editorial%20Complexity%22%3A%20%22Low%22%2C%22NumberofManuscriptPages%22%3A%20%22251%22%7D&amp;redirectURL=https://www.pagemajik.com/&amp;bookDetails=%7B%22categoryName%22%3A%22Production%20and%20Editorial%22%2C%22bookName%22%3A%22%20Arbitration%20%26%20Conciliation%20%22%2C%22chapterCount%22%3A%222%22%2C%20%22isCoverDesignOnly%22%3A%22true%22%7D&amp;userDetails=%7B%22firstName%22%3A%20%22Sulthana%22%2C%22surName%22%3A%20%22S%22%2C%22mailId%22%3A%20%22sulthanas%40s4carlisle.com%22%20%7D</t>
-  </si>
-  <si>
-    <t>http://10.1.6.32/selfpublishing/get_method.php?companyId=11829044757&amp;groupId=11829076861&amp;bookInfo=%7B%22AuthorName%22%3A%20%22John%20Doe%22%2C%22Email%22%3A%20%22JD%40gmail.com%22%2C%22ISBN%22%3A%20%22%22%2C%22Cover%22%3A%20%22Color%22%2C%22Editorial%20Complexity%22%3A%20%22Low%22%2C%22NumberofManuscriptPages%22%3A%20%22251%22%7D&amp;redirectURL=https://www.pagemajik.com/&amp;bookDetails=%7B%22categoryName%22%3A%22Cover%20and%20Production%22%2C%22bookName%22%3A%22%20Arbitration%20%26%20Conciliation%20%22%2C%22chapterCount%22%3A%222%22%2C%20%22isCoverDesignOnly%22%3A%22true%22%7D&amp;userDetails=%7B%22firstName%22%3A%20%22Sulthana%22%2C%22surName%22%3A%20%22S%22%2C%22mailId%22%3A%20%22sulthanas%40s4carlisle.com%22%20%7D</t>
-  </si>
-  <si>
-    <t>http://10.1.6.32/selfpublishing/get_method.php?companyId=11829044757&amp;groupId=11829076861&amp;bookInfo=%7B%22AuthorName%22%3A%20%22John%20Doe%22%2C%22Email%22%3A%20%22JD%40gmail.com%22%2C%22ISBN%22%3A%20%22%22%2C%22Cover%22%3A%20%22Color%22%2C%22Editorial%20Complexity%22%3A%20%22Low%22%2C%22NumberofManuscriptPages%22%3A%20%22251%22%7D&amp;redirectURL=https://www.pagemajik.com/&amp;bookDetails=%7B%22categoryName%22%3A%22Production%2C%C2%A0Editorial%2C%20and%20Index%22%2C%22bookName%22%3A%22%20Arbitration%20%26%20Conciliation%20%22%2C%22chapterCount%22%3A%222%22%2C%20%22isCoverDesignOnly%22%3A%22true%22%7D&amp;userDetails=%7B%22firstName%22%3A%20%22Sulthana%22%2C%22surName%22%3A%20%22S%22%2C%22mailId%22%3A%20%22sulthanas%40s4carlisle.com%22%20%7D</t>
-  </si>
-  <si>
-    <t>http://10.1.6.32/selfpublishing/get_method.php?companyId=11829044757&amp;groupId=11829076861&amp;bookInfo=%7B%22AuthorName%22%3A%20%22John%20Doe%22%2C%22Email%22%3A%20%22JD%40gmail.com%22%2C%22ISBN%22%3A%20%22%22%2C%22Cover%22%3A%20%22Color%22%2C%22Editorial%20Complexity%22%3A%20%22Low%22%2C%22NumberofManuscriptPages%22%3A%20%22251%22%7D&amp;redirectURL=https://www.pagemajik.com/&amp;bookDetails=%7B%22categoryName%22%3A%22Production%2C%20Cover%2C%20and%20Index%22%2C%22bookName%22%3A%22%20Arbitration%20%26%20Conciliation%20%22%2C%22chapterCount%22%3A%222%22%2C%20%22isCoverDesignOnly%22%3A%22true%22%7D&amp;userDetails=%7B%22firstName%22%3A%20%22Sulthana%22%2C%22surName%22%3A%20%22S%22%2C%22mailId%22%3A%20%22sulthanas%40s4carlisle.com%22%20%7D</t>
-  </si>
-  <si>
-    <t>http://10.1.6.32/selfpublishing/get_method.php?companyId=11829044757&amp;groupId=11829076861&amp;bookInfo=%7B%22AuthorName%22%3A%20%22John%20Doe%22%2C%22Email%22%3A%20%22JD%40gmail.com%22%2C%22ISBN%22%3A%20%22%22%2C%22Cover%22%3A%20%22Color%22%2C%22Editorial%20Complexity%22%3A%20%22Low%22%2C%22NumberofManuscriptPages%22%3A%20%22251%22%7D&amp;redirectURL=https://www.pagemajik.com/&amp;bookDetails=%7B%22categoryName%22%3A%22Production%2C%20Cover%2C%20and%20Editorial%22%2C%22bookName%22%3A%22%20Arbitration%20%26%20Conciliation%20%22%2C%22chapterCount%22%3A%222%22%2C%20%22isCoverDesignOnly%22%3A%22true%22%7D&amp;userDetails=%7B%22firstName%22%3A%20%22Sulthana%22%2C%22surName%22%3A%20%22S%22%2C%22mailId%22%3A%20%22sulthanas%40s4carlisle.com%22%20%7D</t>
-  </si>
-  <si>
     <t>Table - services</t>
   </si>
   <si>
     <t>s4c</t>
+  </si>
+  <si>
+    <t>http://10.1.6.32/selfpublishing/get_method.php?companyId=11829044757&amp;groupId=11829076861&amp;bookInfo=%7B%22Author%20Name%22%3A%20%22John%20Doe%22%2C%22Email%22%3A%20%22JD%40gmail.com%22%2C%22ISBN%22%3A%20%22%22%2C%22Cover%22%3A%20%22Color%22%2C%22Editorial%20Complexity%22%3A%20%22Low%22%2C%22Number%20of%20Manuscript%20Pages%22%3A%20%22251%22%7D&amp;redirectURL=https://www.pagemajik.com/&amp;bookDetails=%7B%22categoryName%22%3A%22Full%20Servicess%22%2C%22bookName%22%3A%22%20Arbitration%20%26%20Conciliation%20%22%2C%22chapterCount%22%3A%222%22%2C%20%22isCoverDesignOnly%22%3A%22true%22%7D&amp;userDetails=%7B%22firstName%22%3A%20%22Sulthana%22%2C%22surName%22%3A%20%22S%22%2C%22mailId%22%3A%20%22sulthanas%40s4carlisle.com%22%20%7D</t>
+  </si>
+  <si>
+    <t>http://10.1.6.32/selfpublishing/get_method.php?companyId=11829044757&amp;groupId=11829076861&amp;bookInfo=%7B%22Author%20Name%22%3A%20%22John%20Doe%22%2C%22Email%22%3A%20%22JD%40gmail.com%22%2C%22ISBN%22%3A%20%22%22%2C%22Cover%22%3A%20%22Color%22%2C%22Editorial%20Complexity%22%3A%20%22Low%22%2C%22Number%20of%20Manuscript%20Pages%22%3A%20%22251%22%7D&amp;redirectURL=https://www.pagemajik.com/&amp;bookDetails=%7B%22categoryName%22%3A%22Cover%20Design%22%2C%22bookName%22%3A%22%20Arbitration%20%26%20Conciliation%20%22%2C%22chapterCount%22%3A%222%22%2C%20%22isCoverDesignOnly%22%3A%22true%22%7D&amp;userDetails=%7B%22firstName%22%3A%20%22Sulthana%22%2C%22surName%22%3A%20%22S%22%2C%22mailId%22%3A%20%22sulthanas%40s4carlisle.com%22%20%7D</t>
+  </si>
+  <si>
+    <t>http://10.1.6.32/selfpublishing/get_method.php?companyId=11829044757&amp;groupId=11829076861&amp;bookInfo=%7B%22Author%20Name%22%3A%20%22John%20Doe%22%2C%22Email%22%3A%20%22JD%40gmail.com%22%2C%22ISBN%22%3A%20%22%22%2C%22Cover%22%3A%20%22Color%22%2C%22Editorial%20Complexity%22%3A%20%22Low%22%2C%22Number%20of%20Manuscript%20Pages%22%3A%20%22251%22%7D&amp;redirectURL=https://www.pagemajik.com/&amp;bookDetails=%7B%22categoryName%22%3A%22Production%20Services%22%2C%22bookName%22%3A%22%20Arbitration%20%26%20Conciliation%20%22%2C%22chapterCount%22%3A%222%22%2C%20%22isCoverDesignOnly%22%3A%22true%22%7D&amp;userDetails=%7B%22firstName%22%3A%20%22Sulthana%22%2C%22surName%22%3A%20%22S%22%2C%22mailId%22%3A%20%22sulthanas%40s4carlisle.com%22%20%7D</t>
+  </si>
+  <si>
+    <t>http://10.1.6.32/selfpublishing/get_method.php?companyId=11829044757&amp;groupId=11829076861&amp;bookInfo=%7B%22Author%20Name%22%3A%20%22John%20Doe%22%2C%22Email%22%3A%20%22JD%40gmail.com%22%2C%22ISBN%22%3A%20%22%22%2C%22Cover%22%3A%20%22Color%22%2C%22Editorial%20Complexity%22%3A%20%22Low%22%2C%22Number%20of%20Manuscript%20Pages%22%3A%20%22251%22%7D&amp;redirectURL=https://www.pagemajik.com/&amp;bookDetails=%7B%22categoryName%22%3A%22Editorial%20Services%22%2C%22bookName%22%3A%22%20Arbitration%20%26%20Conciliation%20%22%2C%22chapterCount%22%3A%222%22%2C%20%22isCoverDesignOnly%22%3A%22true%22%7D&amp;userDetails=%7B%22firstName%22%3A%20%22Sulthana%22%2C%22surName%22%3A%20%22S%22%2C%22mailId%22%3A%20%22sulthanas%40s4carlisle.com%22%20%7D</t>
+  </si>
+  <si>
+    <t>http://10.1.6.32/selfpublishing/get_method.php?companyId=11829044757&amp;groupId=11829076861&amp;bookInfo=%7B%22Author%20Name%22%3A%20%22John%20Doe%22%2C%22Email%22%3A%20%22JD%40gmail.com%22%2C%22ISBN%22%3A%20%22%22%2C%22Cover%22%3A%20%22Color%22%2C%22Editorial%20Complexity%22%3A%20%22Low%22%2C%22Number%20of%20Manuscript%20Pages%22%3A%20%22251%22%7D&amp;redirectURL=https://www.pagemajik.com/&amp;bookDetails=%7B%22categoryName%22%3A%22Index%22%2C%22bookName%22%3A%22%20Arbitration%20%26%20Conciliation%20%22%2C%22chapterCount%22%3A%222%22%2C%20%22isCoverDesignOnly%22%3A%22true%22%7D&amp;userDetails=%7B%22firstName%22%3A%20%22Sulthana%22%2C%22surName%22%3A%20%22S%22%2C%22mailId%22%3A%20%22sulthanas%40s4carlisle.com%22%20%7D</t>
+  </si>
+  <si>
+    <t>http://10.1.6.32/selfpublishing/get_method.php?companyId=11829044757&amp;groupId=11829076861&amp;bookInfo=%7B%22Author%20Name%22%3A%20%22John%20Doe%22%2C%22Email%22%3A%20%22JD%40gmail.com%22%2C%22ISBN%22%3A%20%22%22%2C%22Cover%22%3A%20%22Color%22%2C%22Editorial%20Complexity%22%3A%20%22Low%22%2C%22Number%20of%20Manuscript%20Pages%22%3A%20%22251%22%7D&amp;redirectURL=https://www.pagemajik.com/&amp;bookDetails=%7B%22categoryName%22%3A%22Production%20and%20Index%22%2C%22bookName%22%3A%22%20Arbitration%20%26%20Conciliation%20%22%2C%22chapterCount%22%3A%222%22%2C%20%22isCoverDesignOnly%22%3A%22true%22%7D&amp;userDetails=%7B%22firstName%22%3A%20%22Sulthana%22%2C%22surName%22%3A%20%22S%22%2C%22mailId%22%3A%20%22sulthanas%40s4carlisle.com%22%20%7D</t>
+  </si>
+  <si>
+    <t>http://10.1.6.32/selfpublishing/get_method.php?companyId=11829044757&amp;groupId=11829076861&amp;bookInfo=%7B%22Author%20Name%22%3A%20%22John%20Doe%22%2C%22Email%22%3A%20%22JD%40gmail.com%22%2C%22ISBN%22%3A%20%22%22%2C%22Cover%22%3A%20%22Color%22%2C%22Editorial%20Complexity%22%3A%20%22Low%22%2C%22Number%20of%20Manuscript%20Pages%22%3A%20%22251%22%7D&amp;redirectURL=https://www.pagemajik.com/&amp;bookDetails=%7B%22categoryName%22%3A%22Production%20and%20Editorial%22%2C%22bookName%22%3A%22%20Arbitration%20%26%20Conciliation%20%22%2C%22chapterCount%22%3A%222%22%2C%20%22isCoverDesignOnly%22%3A%22true%22%7D&amp;userDetails=%7B%22firstName%22%3A%20%22Sulthana%22%2C%22surName%22%3A%20%22S%22%2C%22mailId%22%3A%20%22sulthanas%40s4carlisle.com%22%20%7D</t>
+  </si>
+  <si>
+    <t>http://10.1.6.32/selfpublishing/get_method.php?companyId=11829044757&amp;groupId=11829076861&amp;bookInfo=%7B%22Author%20Name%22%3A%20%22John%20Doe%22%2C%22Email%22%3A%20%22JD%40gmail.com%22%2C%22ISBN%22%3A%20%22%22%2C%22Cover%22%3A%20%22Color%22%2C%22Editorial%20Complexity%22%3A%20%22Low%22%2C%22Number%20of%20Manuscript%20Pages%22%3A%20%22251%22%7D&amp;redirectURL=https://www.pagemajik.com/&amp;bookDetails=%7B%22categoryName%22%3A%22Cover%20and%20Production%22%2C%22bookName%22%3A%22%20Arbitration%20%26%20Conciliation%20%22%2C%22chapterCount%22%3A%222%22%2C%20%22isCoverDesignOnly%22%3A%22true%22%7D&amp;userDetails=%7B%22firstName%22%3A%20%22Sulthana%22%2C%22surName%22%3A%20%22S%22%2C%22mailId%22%3A%20%22sulthanas%40s4carlisle.com%22%20%7D</t>
+  </si>
+  <si>
+    <t>http://10.1.6.32/selfpublishing/get_method.php?companyId=11829044757&amp;groupId=11829076861&amp;bookInfo=%7B%22Author%20Name%22%3A%20%22John%20Doe%22%2C%22Email%22%3A%20%22JD%40gmail.com%22%2C%22ISBN%22%3A%20%22%22%2C%22Cover%22%3A%20%22Color%22%2C%22Editorial%20Complexity%22%3A%20%22Low%22%2C%22Number%20of%20Manuscript%20Pages%22%3A%20%22251%22%7D&amp;redirectURL=https://www.pagemajik.com/&amp;bookDetails=%7B%22categoryName%22%3A%22Production%2C%C2%A0Editorial%2C%20and%20Index%22%2C%22bookName%22%3A%22%20Arbitration%20%26%20Conciliation%20%22%2C%22chapterCount%22%3A%222%22%2C%20%22isCoverDesignOnly%22%3A%22true%22%7D&amp;userDetails=%7B%22firstName%22%3A%20%22Sulthana%22%2C%22surName%22%3A%20%22S%22%2C%22mailId%22%3A%20%22sulthanas%40s4carlisle.com%22%20%7D</t>
+  </si>
+  <si>
+    <t>http://10.1.6.32/selfpublishing/get_method.php?companyId=11829044757&amp;groupId=11829076861&amp;bookInfo=%7B%22Author%20Name%22%3A%20%22John%20Doe%22%2C%22Email%22%3A%20%22JD%40gmail.com%22%2C%22ISBN%22%3A%20%22%22%2C%22Cover%22%3A%20%22Color%22%2C%22Editorial%20Complexity%22%3A%20%22Low%22%2C%22Number%20of%20Manuscript%20Pages%22%3A%20%22251%22%7D&amp;redirectURL=https://www.pagemajik.com/&amp;bookDetails=%7B%22categoryName%22%3A%22Production%2C%20Cover%2C%20and%20Index%22%2C%22bookName%22%3A%22%20Arbitration%20%26%20Conciliation%20%22%2C%22chapterCount%22%3A%222%22%2C%20%22isCoverDesignOnly%22%3A%22true%22%7D&amp;userDetails=%7B%22firstName%22%3A%20%22Sulthana%22%2C%22surName%22%3A%20%22S%22%2C%22mailId%22%3A%20%22sulthanas%40s4carlisle.com%22%20%7D</t>
+  </si>
+  <si>
+    <t>http://10.1.6.32/selfpublishing/get_method.php?companyId=11829044757&amp;groupId=11829076861&amp;bookInfo=%7B%22Author%20Name%22%3A%20%22John%20Doe%22%2C%22Email%22%3A%20%22JD%40gmail.com%22%2C%22ISBN%22%3A%20%22%22%2C%22Cover%22%3A%20%22Color%22%2C%22Editorial%20Complexity%22%3A%20%22Low%22%2C%22Number%20of%20Manuscript%20Pages%22%3A%20%22251%22%7D&amp;redirectURL=https://www.pagemajik.com/&amp;bookDetails=%7B%22categoryName%22%3A%22Production%2C%20Cover%2C%20and%20Editorial%22%2C%22bookName%22%3A%22%20Arbitration%20%26%20Conciliation%20%22%2C%22chapterCount%22%3A%222%22%2C%20%22isCoverDesignOnly%22%3A%22true%22%7D&amp;userDetails=%7B%22firstName%22%3A%20%22Sulthana%22%2C%22surName%22%3A%20%22S%22%2C%22mailId%22%3A%20%22sulthanas%40s4carlisle.com%22%20%7D</t>
   </si>
 </sst>
 </file>
@@ -884,7 +884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F13" workbookViewId="0">
       <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
@@ -1900,7 +1900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
@@ -1914,10 +1914,10 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="E1" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="F1" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2440,8 +2440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2455,7 +2455,7 @@
         <v>20</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18.75">
@@ -2463,7 +2463,7 @@
         <v>67</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18.75">
@@ -2471,7 +2471,7 @@
         <v>68</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18.75">
@@ -2479,7 +2479,7 @@
         <v>73</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18.75">
@@ -2487,7 +2487,7 @@
         <v>74</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18.75">
@@ -2495,7 +2495,7 @@
         <v>56</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75">
@@ -2503,7 +2503,7 @@
         <v>69</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18.75">
@@ -2511,7 +2511,7 @@
         <v>70</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18.75">
@@ -2519,7 +2519,7 @@
         <v>75</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18.75">
@@ -2527,7 +2527,7 @@
         <v>71</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18.75">
@@ -2535,7 +2535,7 @@
         <v>72</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated isbn validation, added the note for barcode, form disable after submit
</commit_message>
<xml_diff>
--- a/selfPublishing data.xlsx
+++ b/selfPublishing data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="91">
   <si>
     <r>
       <t> </t>
@@ -418,9 +418,6 @@
   </si>
   <si>
     <t>proj_id</t>
-  </si>
-  <si>
-    <t>double</t>
   </si>
   <si>
     <t>template_id</t>
@@ -1910,7 +1907,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1923,10 +1920,10 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="E1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2146,7 +2143,7 @@
         <v>29</v>
       </c>
       <c r="G13" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="H13" t="s">
         <v>45</v>
@@ -2166,7 +2163,7 @@
         <v>30</v>
       </c>
       <c r="G14" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="H14" t="s">
         <v>45</v>
@@ -2186,7 +2183,7 @@
         <v>31</v>
       </c>
       <c r="G15" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="H15" t="s">
         <v>45</v>
@@ -2286,7 +2283,7 @@
         <v>36</v>
       </c>
       <c r="G20" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="H20" t="s">
         <v>45</v>
@@ -2363,7 +2360,7 @@
         <v>45</v>
       </c>
       <c r="F24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G24" t="s">
         <v>41</v>
@@ -2434,23 +2431,23 @@
     </row>
     <row r="28" spans="1:13">
       <c r="F28" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:13">
       <c r="F29" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K29" t="s">
+        <v>64</v>
+      </c>
+      <c r="M29" t="s">
         <v>65</v>
-      </c>
-      <c r="M29" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:13">
       <c r="F30" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2477,39 +2474,39 @@
         <v>20</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18.75">
       <c r="A2" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18.75">
       <c r="A3" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18.75">
       <c r="A4" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18.75">
       <c r="A5" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18.75">
@@ -2517,47 +2514,47 @@
         <v>56</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75">
       <c r="A7" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18.75">
       <c r="A8" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18.75">
       <c r="A9" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18.75">
       <c r="A10" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18.75">
       <c r="A11" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>